<commit_message>
forgot some reaper files
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Desktop\Game Design\Game Design with Unity\GameAudioFinal\IGME-671-Final-Repo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D5039E-0CD4-4550-806C-BD2BBDDA1682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D501268-D748-42E7-8BC0-FAEB17835FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94BD43F3-FAB7-4A99-8189-1BC9B5A900AC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <t>Game Element</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -380,12 +383,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -400,11 +409,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EFAA3A-5326-492A-A19A-600AE3A88855}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,8 +781,8 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>102</v>
+      <c r="F2" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -789,8 +799,8 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>102</v>
+      <c r="F3" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -897,8 +907,8 @@
       <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" t="s">
-        <v>102</v>
+      <c r="F9" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -915,8 +925,8 @@
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
-        <v>102</v>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -938,8 +948,8 @@
       <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="F12" t="s">
-        <v>102</v>
+      <c r="F12" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -956,8 +966,8 @@
       <c r="E13" t="s">
         <v>44</v>
       </c>
-      <c r="F13" t="s">
-        <v>102</v>
+      <c r="F13" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -974,8 +984,8 @@
       <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="F14" t="s">
-        <v>102</v>
+      <c r="F14" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -997,8 +1007,8 @@
       <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="F16" t="s">
-        <v>102</v>
+      <c r="F16" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1015,8 +1025,8 @@
       <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="F17" t="s">
-        <v>102</v>
+      <c r="F17" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1033,8 +1043,8 @@
       <c r="E18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
-        <v>102</v>
+      <c r="F18" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1057,7 +1067,7 @@
         <v>81</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1075,7 +1085,7 @@
         <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1093,7 +1103,7 @@
         <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1111,7 +1121,7 @@
         <v>84</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1134,7 +1144,7 @@
         <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1152,7 +1162,7 @@
         <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1170,7 +1180,7 @@
         <v>87</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1193,7 +1203,7 @@
         <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1211,7 +1221,7 @@
         <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1228,8 +1238,8 @@
       <c r="E31" t="s">
         <v>90</v>
       </c>
-      <c r="F31" t="s">
-        <v>10</v>
+      <c r="F31" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1247,7 +1257,7 @@
         <v>101</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1264,8 +1274,8 @@
       <c r="E33" t="s">
         <v>100</v>
       </c>
-      <c r="F33" t="s">
-        <v>10</v>
+      <c r="F33" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>